<commit_message>
Update CNS length and add PDF to Excel converter
Changed CNS_MIN_LEN to 14 in aih_abas.py. Added a script (pdfto.py) for converting PDF tables to Excel, and included a sample PDF (AIHJAN.pdf). Updated aih_resultados.xlsx, likely reflecting new or processed data.
</commit_message>
<xml_diff>
--- a/Estagio/DadosAbasEspelhoAIH/aih_resultados.xlsx
+++ b/Estagio/DadosAbasEspelhoAIH/aih_resultados.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>280408020407</t>
+          <t>204322025140005</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>100408050896</t>
+          <t>980016286834678</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>140408060379</t>
+          <t>204322025140005</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new abasAIH Excel files and update script input
Added abasAIH3.xlsx through abasAIH7.xlsx to the UnirAbas directory. Updated aih_abas.py to use abasAIH7.xlsx as the input file. Also updated aih_resultados.xlsx with new results.
</commit_message>
<xml_diff>
--- a/Estagio/DadosAbasEspelhoAIH/aih_resultados.xlsx
+++ b/Estagio/DadosAbasEspelhoAIH/aih_resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>312110176572-7</t>
+          <t>312110191680-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -463,14 +463,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>204322013990009</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>312110176572-7</t>
+          <t>312110192110-2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -480,14 +480,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>190149628110005</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>312110176573-8</t>
+          <t>312110192122-3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -497,14 +497,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>204322025140005</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>312110176573-8</t>
+          <t>312110192122-3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -514,14 +514,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>204322025140005</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>312110176573-8</t>
+          <t>312110192147-6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -531,14 +531,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>204322025140005</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>312110177236-0</t>
+          <t>312110192175-1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -548,14 +548,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>204322013990009</t>
+          <t>127980992280001</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>312110177374-6</t>
+          <t>312110192175-1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -572,7 +572,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>312110177374-6</t>
+          <t>312110192175-1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -589,7 +589,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>312110177374-6</t>
+          <t>312110192185-0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -606,7 +606,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>312110177928-0</t>
+          <t>312110192185-0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -623,7 +623,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>312110178135-8</t>
+          <t>312110192185-0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -633,14 +633,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>204322025140005</t>
+          <t>127980992280001</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>312110178136-9</t>
+          <t>312110192204-8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -650,14 +650,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>204322025140005</t>
+          <t>190149628110005</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>312110178676-0</t>
+          <t>312110192204-8</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -667,14 +667,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>705205440440872</t>
+          <t>190149628110005</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>312110178689-1</t>
+          <t>312110192900-0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>312110178738-6</t>
+          <t>312110192901-1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -701,14 +701,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>127980992280001</t>
+          <t>705205440440872</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>312110179538-3</t>
+          <t>312110193161-8</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -718,14 +718,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>980016282340409</t>
+          <t>204322025140005</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>312110179543-8</t>
+          <t>312110193161-8</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -735,14 +735,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>127980992280001</t>
+          <t>204322025140005</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>312110179543-8</t>
+          <t>312110193483-0</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -752,7 +752,194 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>127980992280001</t>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>312110193483-0</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>312110193483-0</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>312110194339-9</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>204322025140005</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>312110194339-9</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>204322025140005</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>312110194953-7</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>204322025140005</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>312110194953-7</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>204322025140005</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>312150252863-9</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>312150252864-0</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>312150252865-0</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>312150252871-6</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>312150252874-9</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>225270</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>980016286834678</t>
         </is>
       </c>
     </row>

</xml_diff>